<commit_message>
test data updated with excel reader.
</commit_message>
<xml_diff>
--- a/src/test/resources/login_test_data.xlsx
+++ b/src/test/resources/login_test_data.xlsx
@@ -9,6 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="homePageData" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="listPurchaseData" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="userCreation" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,12 +23,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">saranya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome admin,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxfest Enterprises PVT LTD,Kochi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diyaninnan+1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diya231</t>
   </si>
 </sst>
 </file>
@@ -35,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -56,6 +80,25 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -112,16 +155,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,7 +191,7 @@
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF2A00FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
@@ -202,18 +253,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -221,7 +272,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -229,20 +280,25 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>809897</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -254,4 +310,117 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.82"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.8"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="Diyaninnan+1@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>